<commit_message>
Update data, fix total summation
</commit_message>
<xml_diff>
--- a/data/zotero_data/bar-graph-classification-sorted.xlsx
+++ b/data/zotero_data/bar-graph-classification-sorted.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tlin/Files/2023-2028 UC Berkeley/_landry-lab/research-project/local/misused-bar-graphs/data/zotero_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33AD38FA-7D4C-7D40-8983-4ABD161AE05B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D3C86A7-703A-4646-99B5-D5CEF218E7FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="500" windowWidth="37620" windowHeight="21100" xr2:uid="{DB5BE922-A247-3047-A984-8AB957C56D7E}"/>
   </bookViews>
@@ -1012,7 +1012,7 @@
   <dimension ref="A1:P15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="134" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1272,13 +1272,13 @@
         <v>38</v>
       </c>
       <c r="G5" s="1">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H5" s="1">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I5" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J5" s="2">
         <f t="shared" si="2"/>
@@ -1298,15 +1298,15 @@
       </c>
       <c r="N5" s="2">
         <f t="shared" si="6"/>
-        <v>18.018018018018019</v>
+        <v>18.918918918918919</v>
       </c>
       <c r="O5" s="2">
         <f t="shared" si="7"/>
-        <v>18.918918918918919</v>
+        <v>19.81981981981982</v>
       </c>
       <c r="P5" s="2">
         <f t="shared" si="8"/>
-        <v>2.7027027027027026</v>
+        <v>3.6036036036036037</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
@@ -1845,64 +1845,64 @@
         <v>16</v>
       </c>
       <c r="B15" s="3">
-        <f>SUM(B5:B14)</f>
-        <v>1596</v>
+        <f>SUM(B2:B14)</f>
+        <v>2250</v>
       </c>
       <c r="C15" s="3">
-        <f>SUM(C5:C14)</f>
-        <v>173</v>
+        <f>SUM(C2:C14)</f>
+        <v>229</v>
       </c>
       <c r="D15" s="3">
         <f t="shared" ref="D15" si="9">B15-C15</f>
-        <v>1423</v>
+        <v>2021</v>
       </c>
       <c r="E15" s="3">
-        <f>SUM(E5:E14)</f>
-        <v>1068</v>
+        <f>SUM(E2:E14)</f>
+        <v>1432</v>
       </c>
       <c r="F15" s="3">
         <f t="shared" ref="F15" si="10">D15-E15</f>
-        <v>355</v>
+        <v>589</v>
       </c>
       <c r="G15" s="3">
-        <f>SUM(G5:G14)</f>
-        <v>205</v>
+        <f>SUM(G2:G14)</f>
+        <v>328</v>
       </c>
       <c r="H15" s="3">
-        <f>SUM(H5:H14)</f>
-        <v>159</v>
+        <f>SUM(H2:H14)</f>
+        <v>276</v>
       </c>
       <c r="I15" s="3">
-        <f>SUM(I5:I14)</f>
-        <v>27</v>
+        <f>SUM(I2:I14)</f>
+        <v>51</v>
       </c>
       <c r="J15" s="4">
         <f t="shared" ref="J15" si="11">C15/B15*100</f>
-        <v>10.839598997493734</v>
+        <v>10.177777777777777</v>
       </c>
       <c r="K15" s="4">
         <f t="shared" ref="K15" si="12">D15/B15*100</f>
-        <v>89.160401002506262</v>
+        <v>89.822222222222223</v>
       </c>
       <c r="L15" s="4">
         <f t="shared" ref="L15" si="13">E15/D15*100</f>
-        <v>75.052705551651442</v>
+        <v>70.85601187530925</v>
       </c>
       <c r="M15" s="4">
         <f t="shared" ref="M15" si="14">F15/D15*100</f>
-        <v>24.947294448348558</v>
+        <v>29.143988124690743</v>
       </c>
       <c r="N15" s="4">
         <f t="shared" ref="N15" si="15">G15/D15*100</f>
-        <v>14.406184118060436</v>
+        <v>16.229589312221673</v>
       </c>
       <c r="O15" s="4">
         <f t="shared" ref="O15" si="16">H15/D15*100</f>
-        <v>11.173576950105412</v>
+        <v>13.656605640771897</v>
       </c>
       <c r="P15" s="4">
         <f t="shared" ref="P15" si="17">I15/D15*100</f>
-        <v>1.8973998594518624</v>
+        <v>2.5235032162295892</v>
       </c>
     </row>
   </sheetData>

</xml_diff>